<commit_message>
add alterações feitas na reunião
</commit_message>
<xml_diff>
--- a/documentação/Ata/modelo.xlsx
+++ b/documentação/Ata/modelo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betis\Documents\FACULDADE ADS\Pesquisa e inovação\projetos\SPRINT-2\sprint-2\Hemolines-Solutions\documentação\Ata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4637e3830c875062/Área de Trabalho/Hemolines Solutions/Hemolines-Solutions/documentação/Ata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8217806A-E841-4E4A-A598-7DD2A6B40B1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{8217806A-E841-4E4A-A598-7DD2A6B40B1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D80447D6-3DD6-4713-A886-4B5E4ABEB27F}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{E0CFAB0B-E106-437F-87A8-EB2711F98D0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E0CFAB0B-E106-437F-87A8-EB2711F98D0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Segunda</t>
   </si>
@@ -62,6 +62,48 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Restruturar banco de dados</t>
+  </si>
+  <si>
+    <t>Itallo</t>
+  </si>
+  <si>
+    <t>home (html)</t>
+  </si>
+  <si>
+    <t>Quem somos (html)</t>
+  </si>
+  <si>
+    <t>Nossa Equipe (html)</t>
+  </si>
+  <si>
+    <t>Guilherme</t>
+  </si>
+  <si>
+    <t>Solução (html)</t>
+  </si>
+  <si>
+    <t>Beatriz</t>
+  </si>
+  <si>
+    <t>Problemas (html)</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Footer (html)</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Iniciado</t>
+  </si>
+  <si>
+    <t>Grupo</t>
   </si>
 </sst>
 </file>
@@ -91,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -137,13 +179,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -155,12 +195,21 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -170,27 +219,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -200,28 +232,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -236,37 +249,17 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -274,44 +267,202 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -322,6 +473,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B3BFE77-DEF8-47FC-AD40-C6E1A3FFBE8B}" name="Tabela1" displayName="Tabela1" ref="A1:D8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:D8" xr:uid="{7F608277-55E4-4440-A9AB-24C5A5D7147B}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0A19CEE3-8DCD-497E-8197-311C5E8D6C04}" name="o que fazer" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{39A8ABF9-630D-4FCB-987F-928609587662}" name="Prazo de entrega" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{22232009-94C6-416F-AAB7-57C48A627CD9}" name="Quem (Responsável)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{DC0B8E70-A608-4CDC-96D7-BF69463D51DE}" name="Status" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F33117D-05DD-4F9C-B5E1-DC7DF9021D21}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,21 +799,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,49 +823,49 @@
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>44281</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>44288</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>44295</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>44302</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>44309</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>44316</v>
       </c>
     </row>
@@ -716,20 +880,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B13174-094E-4DA1-86B7-7ECC223D7E1C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="20" style="20" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
@@ -743,31 +908,114 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="16"/>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="22">
+        <v>44279</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="16"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
+      <c r="A3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="22">
+        <v>44279</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="22">
+        <v>44279</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="22">
+        <v>44279</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="22">
+        <v>44279</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="22">
+        <v>44279</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="26">
+        <v>44279</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>